<commit_message>
add three more capital
</commit_message>
<xml_diff>
--- a/helsinki.xlsx
+++ b/helsinki.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\rendu-data-tp1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul-\Desktop\dossiers\EPSI\data\depot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7031DE18-120A-445D-95EE-14562E6FDA61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFC2EE9-7B1C-41B3-A7E3-96038557D3F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="2460" windowWidth="20910" windowHeight="11835" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SI " sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>janvier</t>
   </si>
@@ -178,12 +178,6 @@
     <t>min /max</t>
   </si>
   <si>
-    <t>identifier les valeurs atypiques ou manquantes</t>
-  </si>
-  <si>
-    <t>définir une méthode pour identifier une valeur atypique</t>
-  </si>
-  <si>
     <t>pour cet échantillon :</t>
   </si>
   <si>
@@ -193,9 +187,6 @@
     <t>Températures moyennes d'une capitale d'Europe</t>
   </si>
   <si>
-    <t>calculer</t>
-  </si>
-  <si>
     <t>par mois</t>
   </si>
   <si>
@@ -215,12 +206,6 @@
   </si>
   <si>
     <t>reprendre les données typiques d'une localisation proche  fournies en complément , comparer les écarts. Qu'en concluez vous ?</t>
-  </si>
-  <si>
-    <t>définir une loi pour valider la pertinence ou non d'une valeur atypique</t>
-  </si>
-  <si>
-    <t>implémenter ces lois dans votre application précédente</t>
   </si>
 </sst>
 </file>
@@ -774,7 +759,7 @@
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -2076,7 +2061,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -2084,7 +2069,7 @@
         <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -2092,7 +2077,7 @@
         <v>46</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -2100,37 +2085,37 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2146,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O99"/>
+  <dimension ref="B1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3339,7 +3324,7 @@
         <v>-1.0555555555555547</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>40</v>
       </c>
@@ -3378,7 +3363,7 @@
         <v>-0.16666666666666705</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>41</v>
       </c>
@@ -3417,7 +3402,7 @@
         <v>-0.38888888888888851</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>42</v>
       </c>
@@ -3446,1628 +3431,6 @@
       <c r="N35" s="1"/>
       <c r="O35">
         <v>-1.5555555555555558</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B60">
-        <f t="shared" ref="B60:B85" si="0">CONVERT(D5,"F","C")</f>
-        <v>-17.407407407407405</v>
-      </c>
-      <c r="C60">
-        <f t="shared" ref="C60:C85" si="1">CONVERT(E5,"F","C")</f>
-        <v>-18.672839506172838</v>
-      </c>
-      <c r="D60">
-        <f t="shared" ref="D60:D85" si="2">CONVERT(F5,"F","C")</f>
-        <v>-26.728395061728396</v>
-      </c>
-      <c r="E60">
-        <f t="shared" ref="E60:E85" si="3">CONVERT(G5,"F","C")</f>
-        <v>-18.827160493827158</v>
-      </c>
-      <c r="F60">
-        <f t="shared" ref="F60:F85" si="4">CONVERT(H5,"F","C")</f>
-        <v>-13.950617283950619</v>
-      </c>
-      <c r="G60">
-        <f t="shared" ref="G60:G85" si="5">CONVERT(I5,"F","C")</f>
-        <v>-8.2098765432098766</v>
-      </c>
-      <c r="H60">
-        <f t="shared" ref="H60:H85" si="6">CONVERT(J5,"F","C")</f>
-        <v>-9.0740740740740726</v>
-      </c>
-      <c r="I60">
-        <f t="shared" ref="I60:I85" si="7">CONVERT(K5,"F","C")</f>
-        <v>-3.9506172839506188</v>
-      </c>
-      <c r="J60">
-        <f t="shared" ref="J60:J85" si="8">CONVERT(L5,"F","C")</f>
-        <v>-8.7345679012345698</v>
-      </c>
-      <c r="K60">
-        <f t="shared" ref="K60:K85" si="9">CONVERT(M5,"F","C")</f>
-        <v>-12.654320987654321</v>
-      </c>
-      <c r="L60">
-        <f t="shared" ref="L60:M60" si="10">CONVERT(N5,"F","C")</f>
-        <v>-13.765432098765432</v>
-      </c>
-      <c r="M60">
-        <f t="shared" si="10"/>
-        <v>-18.641975308641975</v>
-      </c>
-    </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B61">
-        <f t="shared" si="0"/>
-        <v>-15.80246913580247</v>
-      </c>
-      <c r="C61">
-        <f t="shared" si="1"/>
-        <v>-17.314814814814817</v>
-      </c>
-      <c r="D61">
-        <f t="shared" si="2"/>
-        <v>-25.617283950617285</v>
-      </c>
-      <c r="E61">
-        <f t="shared" si="3"/>
-        <v>-18.148148148148145</v>
-      </c>
-      <c r="F61">
-        <f t="shared" si="4"/>
-        <v>-13.703703703703702</v>
-      </c>
-      <c r="G61">
-        <f t="shared" si="5"/>
-        <v>-6.7901234567901252</v>
-      </c>
-      <c r="H61">
-        <f t="shared" si="6"/>
-        <v>-10.679012345679011</v>
-      </c>
-      <c r="I61">
-        <f t="shared" si="7"/>
-        <v>-4.1975308641975317</v>
-      </c>
-      <c r="J61">
-        <f t="shared" si="8"/>
-        <v>-8.9506172839506171</v>
-      </c>
-      <c r="K61">
-        <f t="shared" si="9"/>
-        <v>-13.703703703703702</v>
-      </c>
-      <c r="L61">
-        <f t="shared" ref="L61:M61" si="11">CONVERT(N6,"F","C")</f>
-        <v>-12.901234567901234</v>
-      </c>
-      <c r="M61">
-        <f t="shared" si="11"/>
-        <v>-18.549382716049379</v>
-      </c>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B62">
-        <f t="shared" si="0"/>
-        <v>-16.296296296296298</v>
-      </c>
-      <c r="C62">
-        <f t="shared" si="1"/>
-        <v>-21.358024691358022</v>
-      </c>
-      <c r="D62">
-        <f t="shared" si="2"/>
-        <v>-24.66049382716049</v>
-      </c>
-      <c r="E62">
-        <f t="shared" si="3"/>
-        <v>-18.3641975308642</v>
-      </c>
-      <c r="F62">
-        <f t="shared" si="4"/>
-        <v>-12.932098765432098</v>
-      </c>
-      <c r="G62">
-        <f t="shared" si="5"/>
-        <v>-7.2222222222222223</v>
-      </c>
-      <c r="H62">
-        <f t="shared" si="6"/>
-        <v>-10.679012345679011</v>
-      </c>
-      <c r="I62">
-        <f t="shared" si="7"/>
-        <v>-4.2592592592592595</v>
-      </c>
-      <c r="J62">
-        <f t="shared" si="8"/>
-        <v>-9.0123456790123448</v>
-      </c>
-      <c r="K62">
-        <f t="shared" si="9"/>
-        <v>-14.969135802469134</v>
-      </c>
-      <c r="L62">
-        <f t="shared" ref="L62:M62" si="12">CONVERT(N7,"F","C")</f>
-        <v>-13.67283950617284</v>
-      </c>
-      <c r="M62">
-        <f t="shared" si="12"/>
-        <v>-18.3641975308642</v>
-      </c>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B63">
-        <f t="shared" si="0"/>
-        <v>-58.209876543209873</v>
-      </c>
-      <c r="C63">
-        <f t="shared" si="1"/>
-        <v>-24.043209876543209</v>
-      </c>
-      <c r="D63">
-        <f t="shared" si="2"/>
-        <v>-24.907407407407408</v>
-      </c>
-      <c r="E63">
-        <f t="shared" si="3"/>
-        <v>-18.02469135802469</v>
-      </c>
-      <c r="F63">
-        <f t="shared" si="4"/>
-        <v>-12.746913580246915</v>
-      </c>
-      <c r="G63">
-        <f t="shared" si="5"/>
-        <v>-9.3827160493827133</v>
-      </c>
-      <c r="H63">
-        <f t="shared" si="6"/>
-        <v>-9.1975308641975317</v>
-      </c>
-      <c r="I63">
-        <f t="shared" si="7"/>
-        <v>-6.2654320987654319</v>
-      </c>
-      <c r="J63">
-        <f t="shared" si="8"/>
-        <v>-9.7222222222222214</v>
-      </c>
-      <c r="K63">
-        <f t="shared" si="9"/>
-        <v>-16.358024691358022</v>
-      </c>
-      <c r="L63">
-        <f t="shared" ref="L63:M63" si="13">CONVERT(N8,"F","C")</f>
-        <v>-14.753086419753087</v>
-      </c>
-      <c r="M63">
-        <f t="shared" si="13"/>
-        <v>-15.925925925925926</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B64">
-        <f t="shared" si="0"/>
-        <v>-15.833333333333332</v>
-      </c>
-      <c r="C64">
-        <f t="shared" si="1"/>
-        <v>-22.808641975308642</v>
-      </c>
-      <c r="D64">
-        <f t="shared" si="2"/>
-        <v>-24.382716049382715</v>
-      </c>
-      <c r="E64">
-        <f t="shared" si="3"/>
-        <v>-15.432098765432098</v>
-      </c>
-      <c r="F64">
-        <f t="shared" si="4"/>
-        <v>-12.253086419753087</v>
-      </c>
-      <c r="G64">
-        <f t="shared" si="5"/>
-        <v>-12.56172839506173</v>
-      </c>
-      <c r="H64">
-        <f t="shared" si="6"/>
-        <v>-8.4259259259259256</v>
-      </c>
-      <c r="I64">
-        <f t="shared" si="7"/>
-        <v>-7.2222222222222223</v>
-      </c>
-      <c r="J64">
-        <f t="shared" si="8"/>
-        <v>-9.413580246913579</v>
-      </c>
-      <c r="K64">
-        <f t="shared" si="9"/>
-        <v>-13.734567901234566</v>
-      </c>
-      <c r="L64">
-        <f t="shared" ref="L64:M64" si="14">CONVERT(N9,"F","C")</f>
-        <v>-14.629629629629628</v>
-      </c>
-      <c r="M64">
-        <f t="shared" si="14"/>
-        <v>-16.6358024691358</v>
-      </c>
-    </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65">
-        <f t="shared" si="0"/>
-        <v>-17.006172839506171</v>
-      </c>
-      <c r="C65">
-        <f t="shared" si="1"/>
-        <v>-22.993827160493826</v>
-      </c>
-      <c r="D65">
-        <f t="shared" si="2"/>
-        <v>-21.604938271604937</v>
-      </c>
-      <c r="E65">
-        <f t="shared" si="3"/>
-        <v>-16.327160493827158</v>
-      </c>
-      <c r="F65">
-        <f t="shared" si="4"/>
-        <v>-11.419753086419753</v>
-      </c>
-      <c r="G65">
-        <f t="shared" si="5"/>
-        <v>-12.746913580246915</v>
-      </c>
-      <c r="H65">
-        <f t="shared" si="6"/>
-        <v>-8.2098765432098766</v>
-      </c>
-      <c r="I65">
-        <f t="shared" si="7"/>
-        <v>-8.2098765432098766</v>
-      </c>
-      <c r="J65">
-        <f t="shared" si="8"/>
-        <v>-8.7345679012345698</v>
-      </c>
-      <c r="K65">
-        <f t="shared" si="9"/>
-        <v>-13.364197530864198</v>
-      </c>
-      <c r="L65">
-        <f t="shared" ref="L65:M65" si="15">CONVERT(N10,"F","C")</f>
-        <v>-14.382716049382715</v>
-      </c>
-      <c r="M65">
-        <f t="shared" si="15"/>
-        <v>-19.166666666666668</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66">
-        <f t="shared" si="0"/>
-        <v>-18.919753086419753</v>
-      </c>
-      <c r="C66">
-        <f t="shared" si="1"/>
-        <v>-22.5</v>
-      </c>
-      <c r="D66">
-        <f t="shared" si="2"/>
-        <v>-22.438271604938269</v>
-      </c>
-      <c r="E66">
-        <f t="shared" si="3"/>
-        <v>-16.049382716049383</v>
-      </c>
-      <c r="F66">
-        <f t="shared" si="4"/>
-        <v>-9.7839506172839528</v>
-      </c>
-      <c r="G66">
-        <f t="shared" si="5"/>
-        <v>-11.512345679012345</v>
-      </c>
-      <c r="H66">
-        <f t="shared" si="6"/>
-        <v>-6.4506172839506171</v>
-      </c>
-      <c r="I66">
-        <f t="shared" si="7"/>
-        <v>-7.7160493827160517</v>
-      </c>
-      <c r="J66">
-        <f t="shared" si="8"/>
-        <v>-8.2716049382716044</v>
-      </c>
-      <c r="K66">
-        <f t="shared" si="9"/>
-        <v>-15.216049382716049</v>
-      </c>
-      <c r="L66">
-        <f t="shared" ref="L66:M66" si="16">CONVERT(N11,"F","C")</f>
-        <v>-13.24074074074074</v>
-      </c>
-      <c r="M66">
-        <f t="shared" si="16"/>
-        <v>-17.808641975308642</v>
-      </c>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B67">
-        <f t="shared" si="0"/>
-        <v>-18.734567901234566</v>
-      </c>
-      <c r="C67">
-        <f t="shared" si="1"/>
-        <v>-20.493827160493826</v>
-      </c>
-      <c r="D67">
-        <f t="shared" si="2"/>
-        <v>-20.956790123456788</v>
-      </c>
-      <c r="E67">
-        <f t="shared" si="3"/>
-        <v>-15.277777777777777</v>
-      </c>
-      <c r="F67">
-        <f t="shared" si="4"/>
-        <v>-10.740740740740742</v>
-      </c>
-      <c r="G67">
-        <f t="shared" si="5"/>
-        <v>-11.17283950617284</v>
-      </c>
-      <c r="H67">
-        <f t="shared" si="6"/>
-        <v>-7.9012345679012341</v>
-      </c>
-      <c r="I67">
-        <f t="shared" si="7"/>
-        <v>-7.2530864197530889</v>
-      </c>
-      <c r="J67">
-        <f t="shared" si="8"/>
-        <v>-7.0370370370370372</v>
-      </c>
-      <c r="K67">
-        <f t="shared" si="9"/>
-        <v>-14.938271604938269</v>
-      </c>
-      <c r="L67">
-        <f t="shared" ref="L67:M67" si="17">CONVERT(N12,"F","C")</f>
-        <v>-14.320987654320987</v>
-      </c>
-      <c r="M67">
-        <f t="shared" si="17"/>
-        <v>-17.006172839506171</v>
-      </c>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B68">
-        <f t="shared" si="0"/>
-        <v>-18.24074074074074</v>
-      </c>
-      <c r="C68">
-        <f t="shared" si="1"/>
-        <v>-21.543209876543209</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="2"/>
-        <v>-18.086419753086421</v>
-      </c>
-      <c r="E68">
-        <f t="shared" si="3"/>
-        <v>-14.320987654320987</v>
-      </c>
-      <c r="F68">
-        <f t="shared" si="4"/>
-        <v>-11.388888888888889</v>
-      </c>
-      <c r="G68">
-        <f t="shared" si="5"/>
-        <v>-10.4320987654321</v>
-      </c>
-      <c r="H68">
-        <f t="shared" si="6"/>
-        <v>-7.8086419753086425</v>
-      </c>
-      <c r="I68">
-        <f t="shared" si="7"/>
-        <v>-4.2901234567901225</v>
-      </c>
-      <c r="J68">
-        <f t="shared" si="8"/>
-        <v>-7.9938271604938276</v>
-      </c>
-      <c r="K68">
-        <f t="shared" si="9"/>
-        <v>-11.512345679012345</v>
-      </c>
-      <c r="L68">
-        <f t="shared" ref="L68:M68" si="18">CONVERT(N13,"F","C")</f>
-        <v>-15</v>
-      </c>
-      <c r="M68">
-        <f t="shared" si="18"/>
-        <v>-15.679012345679013</v>
-      </c>
-    </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B69">
-        <f t="shared" si="0"/>
-        <v>-19.62962962962963</v>
-      </c>
-      <c r="C69">
-        <f t="shared" si="1"/>
-        <v>-21.481481481481481</v>
-      </c>
-      <c r="D69">
-        <f t="shared" si="2"/>
-        <v>-17.839506172839506</v>
-      </c>
-      <c r="E69">
-        <f t="shared" si="3"/>
-        <v>-16.481481481481481</v>
-      </c>
-      <c r="F69">
-        <f t="shared" si="4"/>
-        <v>-10.740740740740742</v>
-      </c>
-      <c r="G69">
-        <f t="shared" si="5"/>
-        <v>-9.4753086419753085</v>
-      </c>
-      <c r="H69">
-        <f t="shared" si="6"/>
-        <v>-8.8580246913580254</v>
-      </c>
-      <c r="I69">
-        <f t="shared" si="7"/>
-        <v>-4.9074074074074066</v>
-      </c>
-      <c r="J69">
-        <f t="shared" si="8"/>
-        <v>-8.3641975308641978</v>
-      </c>
-      <c r="K69">
-        <f t="shared" si="9"/>
-        <v>-11.358024691358025</v>
-      </c>
-      <c r="L69">
-        <f t="shared" ref="L69:M69" si="19">CONVERT(N14,"F","C")</f>
-        <v>-15.030864197530864</v>
-      </c>
-      <c r="M69">
-        <f t="shared" si="19"/>
-        <v>-16.666666666666668</v>
-      </c>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70">
-        <f t="shared" si="0"/>
-        <v>-20.061728395061724</v>
-      </c>
-      <c r="C70">
-        <f t="shared" si="1"/>
-        <v>-20.216049382716047</v>
-      </c>
-      <c r="D70">
-        <f t="shared" si="2"/>
-        <v>-17.623456790123456</v>
-      </c>
-      <c r="E70">
-        <f t="shared" si="3"/>
-        <v>-17.654320987654319</v>
-      </c>
-      <c r="F70">
-        <f t="shared" si="4"/>
-        <v>-9.7839506172839528</v>
-      </c>
-      <c r="G70">
-        <f t="shared" si="5"/>
-        <v>-6.7592592592592577</v>
-      </c>
-      <c r="H70">
-        <f t="shared" si="6"/>
-        <v>-7.6543209876543212</v>
-      </c>
-      <c r="I70">
-        <f t="shared" si="7"/>
-        <v>-6.882716049382716</v>
-      </c>
-      <c r="J70">
-        <f t="shared" si="8"/>
-        <v>-9.2592592592592577</v>
-      </c>
-      <c r="K70">
-        <f t="shared" si="9"/>
-        <v>-12.746913580246915</v>
-      </c>
-      <c r="L70">
-        <f t="shared" ref="L70:M70" si="20">CONVERT(N15,"F","C")</f>
-        <v>-15</v>
-      </c>
-      <c r="M70">
-        <f t="shared" si="20"/>
-        <v>-17.438271604938272</v>
-      </c>
-    </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71">
-        <f t="shared" si="0"/>
-        <v>-20</v>
-      </c>
-      <c r="C71">
-        <f t="shared" si="1"/>
-        <v>-19.444444444444443</v>
-      </c>
-      <c r="D71">
-        <f t="shared" si="2"/>
-        <v>-18.086419753086421</v>
-      </c>
-      <c r="E71">
-        <f t="shared" si="3"/>
-        <v>-16.080246913580247</v>
-      </c>
-      <c r="F71">
-        <f t="shared" si="4"/>
-        <v>-9.2901234567901234</v>
-      </c>
-      <c r="G71">
-        <f t="shared" si="5"/>
-        <v>-9.0123456790123448</v>
-      </c>
-      <c r="H71">
-        <f t="shared" si="6"/>
-        <v>-6.5432098765432078</v>
-      </c>
-      <c r="I71">
-        <f t="shared" si="7"/>
-        <v>-9.6913580246913575</v>
-      </c>
-      <c r="J71">
-        <f t="shared" si="8"/>
-        <v>-9.9382716049382722</v>
-      </c>
-      <c r="K71">
-        <f t="shared" si="9"/>
-        <v>-12.098765432098766</v>
-      </c>
-      <c r="L71">
-        <f t="shared" ref="L71:M71" si="21">CONVERT(N16,"F","C")</f>
-        <v>-15</v>
-      </c>
-      <c r="M71">
-        <f t="shared" si="21"/>
-        <v>-17.993827160493826</v>
-      </c>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72">
-        <f t="shared" si="0"/>
-        <v>-19.228395061728396</v>
-      </c>
-      <c r="C72">
-        <f t="shared" si="1"/>
-        <v>-17.962962962962965</v>
-      </c>
-      <c r="D72">
-        <f t="shared" si="2"/>
-        <v>-16.944444444444443</v>
-      </c>
-      <c r="E72">
-        <f t="shared" si="3"/>
-        <v>-15.555555555555555</v>
-      </c>
-      <c r="F72">
-        <f t="shared" si="4"/>
-        <v>-8.3024691358024683</v>
-      </c>
-      <c r="G72">
-        <f t="shared" si="5"/>
-        <v>-9.4753086419753085</v>
-      </c>
-      <c r="H72">
-        <f t="shared" si="6"/>
-        <v>-5.6481481481481488</v>
-      </c>
-      <c r="I72">
-        <f t="shared" si="7"/>
-        <v>-9.5987654320987659</v>
-      </c>
-      <c r="J72">
-        <f t="shared" si="8"/>
-        <v>-10.555555555555555</v>
-      </c>
-      <c r="K72">
-        <f t="shared" si="9"/>
-        <v>-11.234567901234568</v>
-      </c>
-      <c r="L72">
-        <f t="shared" ref="L72:M72" si="22">CONVERT(N17,"F","C")</f>
-        <v>-14.5679012345679</v>
-      </c>
-      <c r="M72">
-        <f t="shared" si="22"/>
-        <v>-19.012345679012345</v>
-      </c>
-    </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B73">
-        <f t="shared" si="0"/>
-        <v>-19.907407407407408</v>
-      </c>
-      <c r="C73">
-        <f t="shared" si="1"/>
-        <v>-17.901234567901234</v>
-      </c>
-      <c r="D73">
-        <f t="shared" si="2"/>
-        <v>-19.413580246913579</v>
-      </c>
-      <c r="E73">
-        <f t="shared" si="3"/>
-        <v>-14.382716049382715</v>
-      </c>
-      <c r="F73">
-        <f t="shared" si="4"/>
-        <v>-6.7283950617283965</v>
-      </c>
-      <c r="G73">
-        <f t="shared" si="5"/>
-        <v>-8.5185185185185173</v>
-      </c>
-      <c r="H73">
-        <f t="shared" si="6"/>
-        <v>-5.3395061728395081</v>
-      </c>
-      <c r="I73">
-        <f t="shared" si="7"/>
-        <v>-8.9197530864197514</v>
-      </c>
-      <c r="J73">
-        <f t="shared" si="8"/>
-        <v>-10.586419753086421</v>
-      </c>
-      <c r="K73">
-        <f t="shared" si="9"/>
-        <v>-10.586419753086421</v>
-      </c>
-      <c r="L73">
-        <f t="shared" ref="L73:M73" si="23">CONVERT(N18,"F","C")</f>
-        <v>-22.098765432098777</v>
-      </c>
-      <c r="M73">
-        <f t="shared" si="23"/>
-        <v>-20.648148148148145</v>
-      </c>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B74">
-        <f t="shared" si="0"/>
-        <v>-21.666666666666668</v>
-      </c>
-      <c r="C74">
-        <f t="shared" si="1"/>
-        <v>-19.938271604938269</v>
-      </c>
-      <c r="D74">
-        <f t="shared" si="2"/>
-        <v>-22.283950617283953</v>
-      </c>
-      <c r="E74">
-        <f t="shared" si="3"/>
-        <v>-14.320987654320987</v>
-      </c>
-      <c r="F74">
-        <f t="shared" si="4"/>
-        <v>-6.5432098765432078</v>
-      </c>
-      <c r="G74">
-        <f t="shared" si="5"/>
-        <v>-8.1172839506172849</v>
-      </c>
-      <c r="H74">
-        <f t="shared" si="6"/>
-        <v>-4.3827160493827142</v>
-      </c>
-      <c r="I74">
-        <f t="shared" si="7"/>
-        <v>-8.9506172839506171</v>
-      </c>
-      <c r="J74">
-        <f t="shared" si="8"/>
-        <v>-10.216049382716049</v>
-      </c>
-      <c r="K74">
-        <f t="shared" si="9"/>
-        <v>-11.018518518518519</v>
-      </c>
-      <c r="L74">
-        <f t="shared" ref="L74:M74" si="24">CONVERT(N19,"F","C")</f>
-        <v>-22.098765432098777</v>
-      </c>
-      <c r="M74">
-        <f t="shared" si="24"/>
-        <v>-21.141975308641975</v>
-      </c>
-    </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B75">
-        <f t="shared" si="0"/>
-        <v>-21.358024691358022</v>
-      </c>
-      <c r="C75">
-        <f t="shared" si="1"/>
-        <v>-20.617283950617285</v>
-      </c>
-      <c r="D75">
-        <f t="shared" si="2"/>
-        <v>-22.530864197530864</v>
-      </c>
-      <c r="E75">
-        <f t="shared" si="3"/>
-        <v>-13.395061728395062</v>
-      </c>
-      <c r="F75">
-        <f t="shared" si="4"/>
-        <v>-7.530864197530863</v>
-      </c>
-      <c r="G75">
-        <f t="shared" si="5"/>
-        <v>-7.9320987654320989</v>
-      </c>
-      <c r="H75">
-        <f t="shared" si="6"/>
-        <v>-3.7654320987654306</v>
-      </c>
-      <c r="I75">
-        <f t="shared" si="7"/>
-        <v>-8.4259259259259256</v>
-      </c>
-      <c r="J75">
-        <f t="shared" si="8"/>
-        <v>-11.296296296296298</v>
-      </c>
-      <c r="K75">
-        <f t="shared" si="9"/>
-        <v>-11.512345679012345</v>
-      </c>
-      <c r="L75">
-        <f t="shared" ref="L75:M75" si="25">CONVERT(N20,"F","C")</f>
-        <v>-12.87037037037037</v>
-      </c>
-      <c r="M75">
-        <f t="shared" si="25"/>
-        <v>-20.154320987654319</v>
-      </c>
-    </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B76">
-        <f t="shared" si="0"/>
-        <v>-21.265432098765434</v>
-      </c>
-      <c r="C76">
-        <f t="shared" si="1"/>
-        <v>-22.067901234567902</v>
-      </c>
-      <c r="D76">
-        <f t="shared" si="2"/>
-        <v>-21.543209876543209</v>
-      </c>
-      <c r="E76">
-        <f t="shared" si="3"/>
-        <v>-13.827160493827162</v>
-      </c>
-      <c r="F76">
-        <f t="shared" si="4"/>
-        <v>-8.4259259259259256</v>
-      </c>
-      <c r="G76">
-        <f t="shared" si="5"/>
-        <v>-7.4382716049382713</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="6"/>
-        <v>-3.6419753086419759</v>
-      </c>
-      <c r="I76">
-        <f t="shared" si="7"/>
-        <v>-7.2530864197530889</v>
-      </c>
-      <c r="J76">
-        <f t="shared" si="8"/>
-        <v>-12.006172839506171</v>
-      </c>
-      <c r="K76">
-        <f t="shared" si="9"/>
-        <v>-11.759259259259258</v>
-      </c>
-      <c r="L76">
-        <f t="shared" ref="L76:M76" si="26">CONVERT(N21,"F","C")</f>
-        <v>-22.098765432098777</v>
-      </c>
-      <c r="M76">
-        <f t="shared" si="26"/>
-        <v>-18.179012345679013</v>
-      </c>
-    </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B77">
-        <f t="shared" si="0"/>
-        <v>-20.216049382716047</v>
-      </c>
-      <c r="C77">
-        <f t="shared" si="1"/>
-        <v>-23.611111111111111</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="2"/>
-        <v>-18.672839506172838</v>
-      </c>
-      <c r="E77">
-        <f t="shared" si="3"/>
-        <v>-12.716049382716049</v>
-      </c>
-      <c r="F77">
-        <f t="shared" si="4"/>
-        <v>-10.092592592592593</v>
-      </c>
-      <c r="G77">
-        <f t="shared" si="5"/>
-        <v>-7.6543209876543212</v>
-      </c>
-      <c r="H77">
-        <f t="shared" si="6"/>
-        <v>-4.32098765432099</v>
-      </c>
-      <c r="I77">
-        <f t="shared" si="7"/>
-        <v>-6.5432098765432078</v>
-      </c>
-      <c r="J77">
-        <f t="shared" si="8"/>
-        <v>-9.6604938271604954</v>
-      </c>
-      <c r="K77">
-        <f t="shared" si="9"/>
-        <v>-11.913580246913579</v>
-      </c>
-      <c r="L77">
-        <f t="shared" ref="L77:M77" si="27">CONVERT(N22,"F","C")</f>
-        <v>-15.709876543209875</v>
-      </c>
-      <c r="M77">
-        <f t="shared" si="27"/>
-        <v>-17.685185185185187</v>
-      </c>
-    </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B78">
-        <f t="shared" si="0"/>
-        <v>-20.339506172839506</v>
-      </c>
-      <c r="C78">
-        <f t="shared" si="1"/>
-        <v>-24.1358024691358</v>
-      </c>
-      <c r="D78">
-        <f t="shared" si="2"/>
-        <v>-17.716049382716047</v>
-      </c>
-      <c r="E78">
-        <f t="shared" si="3"/>
-        <v>-11.975308641975309</v>
-      </c>
-      <c r="F78">
-        <f t="shared" si="4"/>
-        <v>-10.308641975308641</v>
-      </c>
-      <c r="G78">
-        <f t="shared" si="5"/>
-        <v>-9.5679012345679002</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="6"/>
-        <v>-4.6604938271604937</v>
-      </c>
-      <c r="I78">
-        <f t="shared" si="7"/>
-        <v>-7.7469135802469147</v>
-      </c>
-      <c r="J78">
-        <f t="shared" si="8"/>
-        <v>-8.8580246913580254</v>
-      </c>
-      <c r="K78">
-        <f t="shared" si="9"/>
-        <v>-14.351851851851851</v>
-      </c>
-      <c r="L78">
-        <f t="shared" ref="L78:M78" si="28">CONVERT(N23,"F","C")</f>
-        <v>-18.24074074074074</v>
-      </c>
-      <c r="M78">
-        <f t="shared" si="28"/>
-        <v>-17.901234567901234</v>
-      </c>
-    </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B79">
-        <f t="shared" si="0"/>
-        <v>-19.753086419753085</v>
-      </c>
-      <c r="C79">
-        <f t="shared" si="1"/>
-        <v>-24.629629629629626</v>
-      </c>
-      <c r="D79">
-        <f t="shared" si="2"/>
-        <v>-20.185185185185187</v>
-      </c>
-      <c r="E79">
-        <f t="shared" si="3"/>
-        <v>-11.975308641975309</v>
-      </c>
-      <c r="F79">
-        <f t="shared" si="4"/>
-        <v>-9.4753086419753085</v>
-      </c>
-      <c r="G79">
-        <f t="shared" si="5"/>
-        <v>-8.6419753086419746</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="6"/>
-        <v>-6.69753086419753</v>
-      </c>
-      <c r="I79">
-        <f t="shared" si="7"/>
-        <v>-10.030864197530866</v>
-      </c>
-      <c r="J79">
-        <f t="shared" si="8"/>
-        <v>-9.0432098765432105</v>
-      </c>
-      <c r="K79">
-        <f t="shared" si="9"/>
-        <v>-15.432098765432098</v>
-      </c>
-      <c r="L79">
-        <f t="shared" ref="L79:M79" si="29">CONVERT(N24,"F","C")</f>
-        <v>-18.271604938271608</v>
-      </c>
-      <c r="M79">
-        <f t="shared" si="29"/>
-        <v>-20.185185185185187</v>
-      </c>
-    </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B80">
-        <f t="shared" si="0"/>
-        <v>-21.944444444444443</v>
-      </c>
-      <c r="C80">
-        <f t="shared" si="1"/>
-        <v>-26.820987654320987</v>
-      </c>
-      <c r="D80">
-        <f t="shared" si="2"/>
-        <v>-21.141975308641975</v>
-      </c>
-      <c r="E80">
-        <f t="shared" si="3"/>
-        <v>-13.117283950617283</v>
-      </c>
-      <c r="F80">
-        <f t="shared" si="4"/>
-        <v>-8.2098765432098766</v>
-      </c>
-      <c r="G80">
-        <f t="shared" si="5"/>
-        <v>-10.061728395061728</v>
-      </c>
-      <c r="H80">
-        <f t="shared" si="6"/>
-        <v>-5.9876543209876525</v>
-      </c>
-      <c r="I80">
-        <f t="shared" si="7"/>
-        <v>-10.123456790123457</v>
-      </c>
-      <c r="J80">
-        <f t="shared" si="8"/>
-        <v>-8.5493827160493829</v>
-      </c>
-      <c r="K80">
-        <f t="shared" si="9"/>
-        <v>-13.179012345679011</v>
-      </c>
-      <c r="L80">
-        <f t="shared" ref="L80:M80" si="30">CONVERT(N25,"F","C")</f>
-        <v>-18.981481481481481</v>
-      </c>
-      <c r="M80">
-        <f t="shared" si="30"/>
-        <v>-21.728395061728396</v>
-      </c>
-    </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B81">
-        <f t="shared" si="0"/>
-        <v>-22.314814814814813</v>
-      </c>
-      <c r="C81">
-        <f t="shared" si="1"/>
-        <v>-27.561728395061728</v>
-      </c>
-      <c r="D81">
-        <f t="shared" si="2"/>
-        <v>-17.932098765432098</v>
-      </c>
-      <c r="E81">
-        <f t="shared" si="3"/>
-        <v>-15.401234567901234</v>
-      </c>
-      <c r="F81">
-        <f t="shared" si="4"/>
-        <v>-7.9629629629629637</v>
-      </c>
-      <c r="G81">
-        <f t="shared" si="5"/>
-        <v>-11.141975308641976</v>
-      </c>
-      <c r="H81">
-        <f t="shared" si="6"/>
-        <v>-5.5246913580246906</v>
-      </c>
-      <c r="I81">
-        <f t="shared" si="7"/>
-        <v>-9.3209876543209873</v>
-      </c>
-      <c r="J81">
-        <f t="shared" si="8"/>
-        <v>-10.216049382716049</v>
-      </c>
-      <c r="K81">
-        <f t="shared" si="9"/>
-        <v>-12.191358024691358</v>
-      </c>
-      <c r="L81">
-        <f t="shared" ref="L81:M81" si="31">CONVERT(N26,"F","C")</f>
-        <v>-18.302469135802468</v>
-      </c>
-      <c r="M81">
-        <f t="shared" si="31"/>
-        <v>-22.839506172839506</v>
-      </c>
-    </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B82">
-        <f t="shared" si="0"/>
-        <v>-22.345679012345677</v>
-      </c>
-      <c r="C82">
-        <f t="shared" si="1"/>
-        <v>-26.388888888888889</v>
-      </c>
-      <c r="D82">
-        <f t="shared" si="2"/>
-        <v>-19.783950617283953</v>
-      </c>
-      <c r="E82">
-        <f t="shared" si="3"/>
-        <v>-15.771604938271604</v>
-      </c>
-      <c r="F82">
-        <f t="shared" si="4"/>
-        <v>-7.6851851851851842</v>
-      </c>
-      <c r="G82">
-        <f t="shared" si="5"/>
-        <v>-10.061728395061728</v>
-      </c>
-      <c r="H82">
-        <f t="shared" si="6"/>
-        <v>-5.9259259259259247</v>
-      </c>
-      <c r="I82">
-        <f t="shared" si="7"/>
-        <v>-7.5000000000000018</v>
-      </c>
-      <c r="J82">
-        <f t="shared" si="8"/>
-        <v>-11.820987654320987</v>
-      </c>
-      <c r="K82">
-        <f t="shared" si="9"/>
-        <v>-15</v>
-      </c>
-      <c r="L82">
-        <f t="shared" ref="L82:M82" si="32">CONVERT(N27,"F","C")</f>
-        <v>-18.02469135802469</v>
-      </c>
-      <c r="M82">
-        <f t="shared" si="32"/>
-        <v>-23.117283950617285</v>
-      </c>
-    </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B83">
-        <f t="shared" si="0"/>
-        <v>-18.425925925925924</v>
-      </c>
-      <c r="C83">
-        <f t="shared" si="1"/>
-        <v>-26.141975308641975</v>
-      </c>
-      <c r="D83">
-        <f t="shared" si="2"/>
-        <v>-18.518518518518519</v>
-      </c>
-      <c r="E83">
-        <f t="shared" si="3"/>
-        <v>-14.135802469135804</v>
-      </c>
-      <c r="F83">
-        <f t="shared" si="4"/>
-        <v>-9.7222222222222214</v>
-      </c>
-      <c r="G83">
-        <f t="shared" si="5"/>
-        <v>-9.9074074074074083</v>
-      </c>
-      <c r="H83">
-        <f t="shared" si="6"/>
-        <v>-5.3703703703703694</v>
-      </c>
-      <c r="I83">
-        <f t="shared" si="7"/>
-        <v>-7.1604938271604919</v>
-      </c>
-      <c r="J83">
-        <f t="shared" si="8"/>
-        <v>-15.339506172839506</v>
-      </c>
-      <c r="K83">
-        <f t="shared" si="9"/>
-        <v>-15.895061728395062</v>
-      </c>
-      <c r="L83">
-        <f t="shared" ref="L83:M83" si="33">CONVERT(N28,"F","C")</f>
-        <v>-18.425925925925924</v>
-      </c>
-      <c r="M83">
-        <f t="shared" si="33"/>
-        <v>-24.228395061728396</v>
-      </c>
-    </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B84">
-        <f t="shared" si="0"/>
-        <v>-15.524691358024691</v>
-      </c>
-      <c r="C84">
-        <f t="shared" si="1"/>
-        <v>-23.734567901234566</v>
-      </c>
-      <c r="D84">
-        <f t="shared" si="2"/>
-        <v>-16.790123456790123</v>
-      </c>
-      <c r="E84">
-        <f t="shared" si="3"/>
-        <v>-14.197530864197532</v>
-      </c>
-      <c r="F84">
-        <f t="shared" si="4"/>
-        <v>-9.7839506172839528</v>
-      </c>
-      <c r="G84">
-        <f t="shared" si="5"/>
-        <v>-9.4753086419753085</v>
-      </c>
-      <c r="H84">
-        <f t="shared" si="6"/>
-        <v>-4.5679012345679029</v>
-      </c>
-      <c r="I84">
-        <f t="shared" si="7"/>
-        <v>-8.4259259259259256</v>
-      </c>
-      <c r="J84">
-        <f t="shared" si="8"/>
-        <v>-14.074074074074074</v>
-      </c>
-      <c r="K84">
-        <f t="shared" si="9"/>
-        <v>-17.376543209876544</v>
-      </c>
-      <c r="L84">
-        <f t="shared" ref="L84:M84" si="34">CONVERT(N29,"F","C")</f>
-        <v>-20.586419753086421</v>
-      </c>
-      <c r="M84">
-        <f t="shared" si="34"/>
-        <v>-17.654320987654319</v>
-      </c>
-    </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B85">
-        <f t="shared" si="0"/>
-        <v>-16.141975308641975</v>
-      </c>
-      <c r="C85">
-        <f t="shared" si="1"/>
-        <v>-23.734567901234566</v>
-      </c>
-      <c r="D85">
-        <f t="shared" si="2"/>
-        <v>-19.753086419753085</v>
-      </c>
-      <c r="E85">
-        <f t="shared" si="3"/>
-        <v>-14.320987654320987</v>
-      </c>
-      <c r="F85">
-        <f t="shared" si="4"/>
-        <v>-9.7222222222222214</v>
-      </c>
-      <c r="G85">
-        <f t="shared" si="5"/>
-        <v>-8.2098765432098766</v>
-      </c>
-      <c r="H85">
-        <f t="shared" si="6"/>
-        <v>-4.7530864197530853</v>
-      </c>
-      <c r="I85">
-        <f t="shared" si="7"/>
-        <v>-9.5987654320987659</v>
-      </c>
-      <c r="J85">
-        <f t="shared" si="8"/>
-        <v>-12.407407407407408</v>
-      </c>
-      <c r="K85">
-        <f t="shared" si="9"/>
-        <v>-16.944444444444443</v>
-      </c>
-      <c r="L85">
-        <f t="shared" ref="L85:M85" si="35">CONVERT(N30,"F","C")</f>
-        <v>-19.722222222222221</v>
-      </c>
-      <c r="M85">
-        <f t="shared" si="35"/>
-        <v>-17.469135802469136</v>
-      </c>
-    </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B86">
-        <f>CONVERT(D31,"F","C")</f>
-        <v>-16.882716049382715</v>
-      </c>
-      <c r="D86">
-        <f t="shared" ref="D86:K89" si="36">CONVERT(F31,"F","C")</f>
-        <v>-20.895061728395063</v>
-      </c>
-      <c r="E86">
-        <f t="shared" si="36"/>
-        <v>-14.938271604938269</v>
-      </c>
-      <c r="F86">
-        <f t="shared" si="36"/>
-        <v>-8.6728395061728385</v>
-      </c>
-      <c r="G86">
-        <f t="shared" si="36"/>
-        <v>-6.882716049382716</v>
-      </c>
-      <c r="H86">
-        <f t="shared" si="36"/>
-        <v>-4.3827160493827142</v>
-      </c>
-      <c r="I86">
-        <f t="shared" si="36"/>
-        <v>-9.5987654320987659</v>
-      </c>
-      <c r="J86">
-        <f t="shared" si="36"/>
-        <v>-12.962962962962962</v>
-      </c>
-      <c r="K86">
-        <f t="shared" si="36"/>
-        <v>-17.438271604938272</v>
-      </c>
-      <c r="L86">
-        <f t="shared" ref="L86:M86" si="37">CONVERT(N31,"F","C")</f>
-        <v>-20.246913580246911</v>
-      </c>
-      <c r="M86">
-        <f t="shared" si="37"/>
-        <v>-18.271604938271608</v>
-      </c>
-    </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B87">
-        <f>CONVERT(D32,"F","C")</f>
-        <v>-17.962962962962965</v>
-      </c>
-      <c r="D87">
-        <f t="shared" si="36"/>
-        <v>-19.969135802469136</v>
-      </c>
-      <c r="E87">
-        <f t="shared" si="36"/>
-        <v>-14.012345679012345</v>
-      </c>
-      <c r="F87">
-        <f t="shared" si="36"/>
-        <v>-8.6728395061728385</v>
-      </c>
-      <c r="G87">
-        <f t="shared" si="36"/>
-        <v>-6.3271604938271624</v>
-      </c>
-      <c r="H87">
-        <f t="shared" si="36"/>
-        <v>-4.0740740740740735</v>
-      </c>
-      <c r="I87">
-        <f t="shared" si="36"/>
-        <v>-9.5987654320987659</v>
-      </c>
-      <c r="J87">
-        <f t="shared" si="36"/>
-        <v>-14.320987654320987</v>
-      </c>
-      <c r="K87">
-        <f t="shared" si="36"/>
-        <v>-18.179012345679013</v>
-      </c>
-      <c r="L87">
-        <f t="shared" ref="L87:M87" si="38">CONVERT(N32,"F","C")</f>
-        <v>-20.833333333333332</v>
-      </c>
-      <c r="M87">
-        <f t="shared" si="38"/>
-        <v>-18.3641975308642</v>
-      </c>
-    </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B88">
-        <f>CONVERT(D33,"F","C")</f>
-        <v>-17.962962962962965</v>
-      </c>
-      <c r="D88">
-        <f t="shared" si="36"/>
-        <v>-19.691358024691358</v>
-      </c>
-      <c r="E88">
-        <f t="shared" si="36"/>
-        <v>-14.320987654320987</v>
-      </c>
-      <c r="F88">
-        <f t="shared" si="36"/>
-        <v>-7.1604938271604919</v>
-      </c>
-      <c r="G88">
-        <f t="shared" si="36"/>
-        <v>-10.092592592592593</v>
-      </c>
-      <c r="H88">
-        <f t="shared" si="36"/>
-        <v>-4.0432098765432105</v>
-      </c>
-      <c r="I88">
-        <f t="shared" si="36"/>
-        <v>-9.2901234567901234</v>
-      </c>
-      <c r="J88">
-        <f t="shared" si="36"/>
-        <v>-14.845679012345679</v>
-      </c>
-      <c r="K88">
-        <f t="shared" si="36"/>
-        <v>-18.919753086419753</v>
-      </c>
-      <c r="L88">
-        <f t="shared" ref="L88:M88" si="39">CONVERT(N33,"F","C")</f>
-        <v>-18.055555555555554</v>
-      </c>
-      <c r="M88">
-        <f t="shared" si="39"/>
-        <v>-17.87037037037037</v>
-      </c>
-    </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B89">
-        <f>CONVERT(D34,"F","C")</f>
-        <v>-19.598765432098766</v>
-      </c>
-      <c r="D89">
-        <f t="shared" si="36"/>
-        <v>-20</v>
-      </c>
-      <c r="E89">
-        <f t="shared" si="36"/>
-        <v>-13.611111111111111</v>
-      </c>
-      <c r="F89">
-        <f t="shared" si="36"/>
-        <v>-7.7160493827160517</v>
-      </c>
-      <c r="G89">
-        <f t="shared" si="36"/>
-        <v>-10.339506172839506</v>
-      </c>
-      <c r="H89">
-        <f t="shared" si="36"/>
-        <v>-4.1049382716049401</v>
-      </c>
-      <c r="I89">
-        <f t="shared" si="36"/>
-        <v>-9.7530864197530871</v>
-      </c>
-      <c r="J89">
-        <f t="shared" si="36"/>
-        <v>-12.469135802469134</v>
-      </c>
-      <c r="K89">
-        <f t="shared" si="36"/>
-        <v>-16.172839506172838</v>
-      </c>
-      <c r="L89">
-        <f t="shared" ref="L89:M89" si="40">CONVERT(N34,"F","C")</f>
-        <v>-17.376543209876544</v>
-      </c>
-      <c r="M89">
-        <f t="shared" si="40"/>
-        <v>-17.993827160493826</v>
-      </c>
-    </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B90">
-        <f>CONVERT(D35,"F","C")</f>
-        <v>-20.030864197530864</v>
-      </c>
-      <c r="D90">
-        <f>CONVERT(F35,"F","C")</f>
-        <v>-19.537037037037035</v>
-      </c>
-      <c r="F90">
-        <f>CONVERT(H35,"F","C")</f>
-        <v>-9.8148148148148149</v>
-      </c>
-      <c r="H90">
-        <f>CONVERT(J35,"F","C")</f>
-        <v>-4.0740740740740735</v>
-      </c>
-      <c r="I90">
-        <f>CONVERT(K35,"F","C")</f>
-        <v>-9.0123456790123448</v>
-      </c>
-      <c r="K90">
-        <f>CONVERT(M35,"F","C")</f>
-        <v>-13.641975308641976</v>
-      </c>
-      <c r="M90">
-        <f t="shared" ref="M90" si="41">CONVERT(O35,"F","C")</f>
-        <v>-18.641975308641975</v>
-      </c>
-    </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F94" t="str">
-        <f t="shared" ref="F94:F99" si="42">REPLACE(G38,1,34,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F95" t="str">
-        <f t="shared" si="42"/>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F96" t="str">
-        <f t="shared" si="42"/>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F97" t="str">
-        <f t="shared" si="42"/>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F98" t="str">
-        <f t="shared" si="42"/>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F99" t="str">
-        <f t="shared" si="42"/>
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>